<commit_message>
- comentando parte que salva pre-processadas em pasta
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF15D89-237F-43FD-B6BC-7D4C524246C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0B3F53-8236-448F-845C-0DBCFFDBD070}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -31,19 +31,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>imagem</t>
   </si>
   <si>
     <t>knn</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>svm</t>
+  </si>
+  <si>
+    <t>04_R_N_H_P</t>
+  </si>
+  <si>
+    <t>08_R_N_L_P</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Preprocessada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,16 +72,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -68,17 +102,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -89,6 +151,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3D6F540-399B-496E-BBAB-6751E98C60EF}" name="Tabela3" displayName="Tabela3" ref="A2:D10" totalsRowShown="0">
+  <autoFilter ref="A2:D10" xr:uid="{0B87829A-877F-4382-85ED-EEE53BEC3019}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{08257DDB-CB06-4C42-8B0D-2937C730D845}" name="imagem"/>
+    <tableColumn id="2" xr3:uid="{434A72B2-A753-49CF-882E-43BC9930B322}" name="knn" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7BFFDED5-C7DD-47D9-8C59-C46507B7E44C}" name="tree"/>
+    <tableColumn id="4" xr3:uid="{0FF6ECD6-FE45-4460-AF88-0E8DCE28F784}" name="svm"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A9A58D94-9E18-417C-86F9-C2E6F6C71EED}" name="Tabela35" displayName="Tabela35" ref="A13:D20" totalsRowShown="0">
+  <autoFilter ref="A13:D20" xr:uid="{74F37799-3BFF-4C54-9FBD-ED00B98311E5}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{994470AB-8167-49CA-AFE5-8BC377B926F9}" name="imagem"/>
+    <tableColumn id="2" xr3:uid="{9A1646D8-E8B9-445E-8EE9-99E7F61BD1CD}" name="knn" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{5E67CCD2-5ABE-4BC7-9E72-60C12FA94D9C}" name="tree"/>
+    <tableColumn id="4" xr3:uid="{D51E5E27-D86D-47BA-BFC5-F3347C9C230E}" name="svm"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,23 +476,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>63.157800000000002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>63.157800000000002</v>
+      </c>
+      <c r="D3" s="1">
+        <v>63.157800000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>63.157800000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <v>63.157800000000002</v>
+      </c>
+      <c r="D4" s="1">
+        <v>63.157800000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>60.526299999999999</v>
+      </c>
+      <c r="C14" s="1">
+        <v>63.157800000000002</v>
+      </c>
+      <c r="D14" s="1">
+        <v>63.157800000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A12:D12"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Markpoint Projeto: Idade e Sexo
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0B3F53-8236-448F-845C-0DBCFFDBD070}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C31FC3-180F-4681-AB1A-6533941879D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>imagem</t>
   </si>
@@ -55,6 +55,39 @@
   </si>
   <si>
     <t>Preprocessada</t>
+  </si>
+  <si>
+    <t>treinamento</t>
+  </si>
+  <si>
+    <t>63 h</t>
+  </si>
+  <si>
+    <t>24 m</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>30 h</t>
+  </si>
+  <si>
+    <t>8 m</t>
+  </si>
+  <si>
+    <t>relação</t>
+  </si>
+  <si>
+    <t>0,4761904761904762‬</t>
+  </si>
+  <si>
+    <t>0,3333333333333333‬</t>
+  </si>
+  <si>
+    <t>rng(5)</t>
+  </si>
+  <si>
+    <t>16_L_N_L_BH</t>
   </si>
 </sst>
 </file>
@@ -62,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -122,10 +155,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -133,12 +170,18 @@
     <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -158,7 +201,7 @@
   <autoFilter ref="A2:D10" xr:uid="{0B87829A-877F-4382-85ED-EEE53BEC3019}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{08257DDB-CB06-4C42-8B0D-2937C730D845}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{434A72B2-A753-49CF-882E-43BC9930B322}" name="knn" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{434A72B2-A753-49CF-882E-43BC9930B322}" name="knn" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{7BFFDED5-C7DD-47D9-8C59-C46507B7E44C}" name="tree"/>
     <tableColumn id="4" xr3:uid="{0FF6ECD6-FE45-4460-AF88-0E8DCE28F784}" name="svm"/>
   </tableColumns>
@@ -171,9 +214,35 @@
   <autoFilter ref="A13:D20" xr:uid="{74F37799-3BFF-4C54-9FBD-ED00B98311E5}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{994470AB-8167-49CA-AFE5-8BC377B926F9}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{9A1646D8-E8B9-445E-8EE9-99E7F61BD1CD}" name="knn" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{9A1646D8-E8B9-445E-8EE9-99E7F61BD1CD}" name="knn" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{5E67CCD2-5ABE-4BC7-9E72-60C12FA94D9C}" name="tree"/>
     <tableColumn id="4" xr3:uid="{D51E5E27-D86D-47BA-BFC5-F3347C9C230E}" name="svm"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EEF2306-E820-4CE8-979C-C6FB52CD2FD5}" name="Tabela32" displayName="Tabela32" ref="G7:J15" totalsRowShown="0">
+  <autoFilter ref="G7:J15" xr:uid="{EB878039-24AA-41C0-A2E9-CE86D283C241}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{9CD6EEAF-D605-4188-A062-2821793F7914}" name="imagem"/>
+    <tableColumn id="2" xr3:uid="{2134A55D-67F8-4BDE-B2FF-785EF61F65A6}" name="knn" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{3887058B-F545-4BEC-89FF-1A68324FCC0A}" name="tree"/>
+    <tableColumn id="4" xr3:uid="{3CE57E63-AE1A-4E11-9613-94E7EEAAA591}" name="svm"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DBCEC551-9AAE-4DA6-A13B-39071F740BB4}" name="Tabela323" displayName="Tabela323" ref="G18:J26" totalsRowShown="0">
+  <autoFilter ref="G18:J26" xr:uid="{1CEBC6BA-CB92-44A6-93B4-15A4EA0244E8}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B7A0FF2E-054F-456E-870A-FF3A260F7146}" name="imagem"/>
+    <tableColumn id="2" xr3:uid="{3C8D1900-8F47-4840-B8D7-322F97FDFF17}" name="knn" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{FC4CE911-627D-4E58-AF6A-A13B3C4050AB}" name="tree"/>
+    <tableColumn id="4" xr3:uid="{1CC04F71-0C11-4F0F-AF8E-4F819652D39C}" name="svm"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -476,27 +545,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -509,8 +588,17 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -523,8 +611,17 @@
       <c r="D3" s="1">
         <v>63.157800000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -537,35 +634,101 @@
       <c r="D4" s="1">
         <v>63.157800000000002</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>71.052599999999998</v>
+      </c>
+      <c r="I8" s="1">
+        <v>78.947400000000002</v>
+      </c>
+      <c r="J8" s="1">
+        <v>78.947400000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>73.684200000000004</v>
+      </c>
+      <c r="I9" s="1">
+        <v>78.947400000000002</v>
+      </c>
+      <c r="J9" s="1">
+        <v>78.947400000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="1">
+        <v>73.684200000000004</v>
+      </c>
+      <c r="I10" s="1">
+        <v>78.947400000000002</v>
+      </c>
+      <c r="J10" s="1">
+        <v>78.947400000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -578,48 +741,116 @@
       <c r="D13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1">
-        <v>60.526299999999999</v>
+        <v>63.157899999999998</v>
       </c>
       <c r="C14" s="1">
-        <v>63.157800000000002</v>
+        <v>63.157899999999998</v>
       </c>
       <c r="D14" s="1">
-        <v>63.157800000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63.157899999999998</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="1">
+        <v>78.947400000000002</v>
+      </c>
+      <c r="I21" s="1">
+        <v>78.947400000000002</v>
+      </c>
+      <c r="J21" s="1">
+        <v>78.947400000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
+    <mergeCell ref="G17:J17"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Mudança para obtenção para ImageDatastore - Classificação utilizando SVM multiclasses - Ajuste em observações - Ajuste em estatísticas - Armazenamento de workspace com feature extraction das imagem de treinamento e teste. - Acurácia com SVM sem otimização de 0.9813
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C31FC3-180F-4681-AB1A-6533941879D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A59847D-8809-4D2B-98AD-3C4CBFE9A13E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>imagem</t>
   </si>
@@ -57,37 +57,10 @@
     <t>Preprocessada</t>
   </si>
   <si>
-    <t>treinamento</t>
-  </si>
-  <si>
-    <t>63 h</t>
-  </si>
-  <si>
-    <t>24 m</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>30 h</t>
-  </si>
-  <si>
-    <t>8 m</t>
-  </si>
-  <si>
-    <t>relação</t>
-  </si>
-  <si>
-    <t>0,4761904761904762‬</t>
-  </si>
-  <si>
-    <t>0,3333333333333333‬</t>
-  </si>
-  <si>
-    <t>rng(5)</t>
-  </si>
-  <si>
     <t>16_L_N_L_BH</t>
+  </si>
+  <si>
+    <t>0.9813</t>
   </si>
 </sst>
 </file>
@@ -155,14 +128,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -170,13 +139,7 @@
     <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -197,32 +160,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3D6F540-399B-496E-BBAB-6751E98C60EF}" name="Tabela3" displayName="Tabela3" ref="A2:D10" totalsRowShown="0">
-  <autoFilter ref="A2:D10" xr:uid="{0B87829A-877F-4382-85ED-EEE53BEC3019}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{08257DDB-CB06-4C42-8B0D-2937C730D845}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{434A72B2-A753-49CF-882E-43BC9930B322}" name="knn" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{7BFFDED5-C7DD-47D9-8C59-C46507B7E44C}" name="tree"/>
-    <tableColumn id="4" xr3:uid="{0FF6ECD6-FE45-4460-AF88-0E8DCE28F784}" name="svm"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A9A58D94-9E18-417C-86F9-C2E6F6C71EED}" name="Tabela35" displayName="Tabela35" ref="A13:D20" totalsRowShown="0">
-  <autoFilter ref="A13:D20" xr:uid="{74F37799-3BFF-4C54-9FBD-ED00B98311E5}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{994470AB-8167-49CA-AFE5-8BC377B926F9}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{9A1646D8-E8B9-445E-8EE9-99E7F61BD1CD}" name="knn" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{5E67CCD2-5ABE-4BC7-9E72-60C12FA94D9C}" name="tree"/>
-    <tableColumn id="4" xr3:uid="{D51E5E27-D86D-47BA-BFC5-F3347C9C230E}" name="svm"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EEF2306-E820-4CE8-979C-C6FB52CD2FD5}" name="Tabela32" displayName="Tabela32" ref="G7:J15" totalsRowShown="0">
   <autoFilter ref="G7:J15" xr:uid="{EB878039-24AA-41C0-A2E9-CE86D283C241}"/>
   <tableColumns count="4">
@@ -235,7 +172,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DBCEC551-9AAE-4DA6-A13B-39071F740BB4}" name="Tabela323" displayName="Tabela323" ref="G18:J26" totalsRowShown="0">
   <autoFilter ref="G18:J26" xr:uid="{1CEBC6BA-CB92-44A6-93B4-15A4EA0244E8}"/>
   <tableColumns count="4">
@@ -545,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="G5:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,94 +498,8 @@
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="G1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>63.157800000000002</v>
-      </c>
-      <c r="C3" s="1">
-        <v>63.157800000000002</v>
-      </c>
-      <c r="D3" s="1">
-        <v>63.157800000000002</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>63.157800000000002</v>
-      </c>
-      <c r="C4" s="1">
-        <v>63.157800000000002</v>
-      </c>
-      <c r="D4" s="1">
-        <v>63.157800000000002</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
+    <row r="5" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="7:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
@@ -656,8 +507,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+    <row r="7" spans="7:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>0</v>
       </c>
@@ -671,102 +521,49 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+    <row r="8" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="1">
-        <v>71.052599999999998</v>
-      </c>
-      <c r="I8" s="1">
-        <v>78.947400000000002</v>
-      </c>
-      <c r="J8" s="1">
-        <v>78.947400000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="1">
-        <v>73.684200000000004</v>
-      </c>
-      <c r="I9" s="1">
-        <v>78.947400000000002</v>
-      </c>
-      <c r="J9" s="1">
-        <v>78.947400000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="1">
-        <v>73.684200000000004</v>
-      </c>
-      <c r="I10" s="1">
-        <v>78.947400000000002</v>
-      </c>
-      <c r="J10" s="1">
-        <v>78.947400000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+    <row r="12" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
+    <row r="13" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1">
-        <v>63.157899999999998</v>
-      </c>
-      <c r="C14" s="1">
-        <v>63.157899999999998</v>
-      </c>
-      <c r="D14" s="1">
-        <v>63.157899999999998</v>
-      </c>
+    <row r="14" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
+    <row r="15" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
+    <row r="16" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="7:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G17" s="2" t="s">
         <v>7</v>
       </c>
@@ -774,8 +571,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+    <row r="18" spans="7:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>0</v>
       </c>
@@ -789,8 +585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
         <v>4</v>
       </c>
@@ -798,8 +593,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
         <v>5</v>
       </c>
@@ -807,50 +601,39 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="1">
-        <v>78.947400000000002</v>
-      </c>
-      <c r="I21" s="1">
-        <v>78.947400000000002</v>
-      </c>
-      <c r="J21" s="1">
-        <v>78.947400000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="G17:J17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A12:D12"/>
     <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G1:J1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Otimização do SVM - Atualização em estatísticas
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A59847D-8809-4D2B-98AD-3C4CBFE9A13E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D8995-1087-4286-80C9-973EA0AD3CB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>16_L_N_L_BH</t>
   </si>
   <si>
-    <t>0.9813</t>
+    <t>0.9875</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="G5:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Geração de resultados - Alteração de estatísticas
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D8995-1087-4286-80C9-973EA0AD3CB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7733779-0F42-4E8D-9AC2-EB4570E49ACA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>imagem</t>
   </si>
@@ -51,16 +51,103 @@
     <t>08_R_N_L_P</t>
   </si>
   <si>
-    <t>Original</t>
-  </si>
-  <si>
-    <t>Preprocessada</t>
-  </si>
-  <si>
     <t>16_L_N_L_BH</t>
   </si>
   <si>
     <t>0.9875</t>
+  </si>
+  <si>
+    <t>NIR</t>
+  </si>
+  <si>
+    <t>Sem Pré-processamento</t>
+  </si>
+  <si>
+    <t>knn2</t>
+  </si>
+  <si>
+    <t>tree3</t>
+  </si>
+  <si>
+    <t>svm4</t>
+  </si>
+  <si>
+    <t>Com Pré-processamento</t>
+  </si>
+  <si>
+    <t>02_R_N_H_BH</t>
+  </si>
+  <si>
+    <t>06_R_N_L_BH</t>
+  </si>
+  <si>
+    <t>09_R_N_L_W</t>
+  </si>
+  <si>
+    <t>14_L_N_H_P</t>
+  </si>
+  <si>
+    <t>12_L_N_H_BH</t>
+  </si>
+  <si>
+    <t>18_L_N_L_P</t>
+  </si>
+  <si>
+    <t>19_L_N_L_W</t>
+  </si>
+  <si>
+    <t>VISÍVEL</t>
+  </si>
+  <si>
+    <t>01_R_V_H_BH</t>
+  </si>
+  <si>
+    <t>03_R_V_H_P</t>
+  </si>
+  <si>
+    <t>05_R_V_L_BH</t>
+  </si>
+  <si>
+    <t>07_R_V_L_P</t>
+  </si>
+  <si>
+    <t>10_R_V_L_W</t>
+  </si>
+  <si>
+    <t>11_L_V_H_BH</t>
+  </si>
+  <si>
+    <t>13_L_V_H_P</t>
+  </si>
+  <si>
+    <t>15_L_V_L_BH</t>
+  </si>
+  <si>
+    <t>17_L_V_L_P</t>
+  </si>
+  <si>
+    <t>20_L_V_L_W</t>
+  </si>
+  <si>
+    <t>0.9688</t>
+  </si>
+  <si>
+    <t>0.9625</t>
+  </si>
+  <si>
+    <t>0.9938</t>
+  </si>
+  <si>
+    <t>0.9876</t>
+  </si>
+  <si>
+    <t>0.9813</t>
+  </si>
+  <si>
+    <t>0.9563</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
 </sst>
 </file>
@@ -100,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -123,15 +210,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -139,7 +261,16 @@
     <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -160,26 +291,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EEF2306-E820-4CE8-979C-C6FB52CD2FD5}" name="Tabela32" displayName="Tabela32" ref="G7:J15" totalsRowShown="0">
-  <autoFilter ref="G7:J15" xr:uid="{EB878039-24AA-41C0-A2E9-CE86D283C241}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1EEF2306-E820-4CE8-979C-C6FB52CD2FD5}" name="Tabela32" displayName="Tabela32" ref="A3:G13" totalsRowShown="0">
+  <autoFilter ref="A3:G13" xr:uid="{EB878039-24AA-41C0-A2E9-CE86D283C241}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:G13">
+    <sortCondition ref="A4"/>
+  </sortState>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9CD6EEAF-D605-4188-A062-2821793F7914}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{2134A55D-67F8-4BDE-B2FF-785EF61F65A6}" name="knn" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{2134A55D-67F8-4BDE-B2FF-785EF61F65A6}" name="knn" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{3887058B-F545-4BEC-89FF-1A68324FCC0A}" name="tree"/>
-    <tableColumn id="4" xr3:uid="{3CE57E63-AE1A-4E11-9613-94E7EEAAA591}" name="svm"/>
+    <tableColumn id="4" xr3:uid="{3CE57E63-AE1A-4E11-9613-94E7EEAAA591}" name="svm" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{EE35EF4B-7DC7-4E69-86C3-451405342ABC}" name="knn2" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7433D010-4521-40A5-BA92-1C0C0211473F}" name="tree3"/>
+    <tableColumn id="7" xr3:uid="{6B5FDDCA-D14F-4A1D-B8C4-0EED1F96B1C6}" name="svm4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DBCEC551-9AAE-4DA6-A13B-39071F740BB4}" name="Tabela323" displayName="Tabela323" ref="G18:J26" totalsRowShown="0">
-  <autoFilter ref="G18:J26" xr:uid="{1CEBC6BA-CB92-44A6-93B4-15A4EA0244E8}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B7A0FF2E-054F-456E-870A-FF3A260F7146}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{3C8D1900-8F47-4840-B8D7-322F97FDFF17}" name="knn" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{FC4CE911-627D-4E58-AF6A-A13B3C4050AB}" name="tree"/>
-    <tableColumn id="4" xr3:uid="{1CC04F71-0C11-4F0F-AF8E-4F819652D39C}" name="svm"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{14CD7A79-EBA2-403E-89F1-36C06DE30360}" name="Tabela323" displayName="Tabela323" ref="A17:G27" totalsRowShown="0">
+  <autoFilter ref="A17:G27" xr:uid="{003B4969-11A4-4A46-9CA1-96A2091FBFC8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:G26">
+    <sortCondition ref="A4"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{CC27BF8B-77D1-448F-8209-CAD32532EAEE}" name="imagem"/>
+    <tableColumn id="2" xr3:uid="{4917905F-B362-479A-93E9-7F422DD76BBA}" name="knn" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F84F7CF0-9FAA-4375-A3B1-2AE4D8D3E70E}" name="tree"/>
+    <tableColumn id="4" xr3:uid="{7F13AB8D-1286-4F3C-90FD-05FABB5D6375}" name="svm"/>
+    <tableColumn id="5" xr3:uid="{3CD7279F-C579-45B8-AE64-9F1FFE66FFCB}" name="knn2" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{B08DF77A-B16A-4D9C-A83C-C127469C2282}" name="tree3"/>
+    <tableColumn id="7" xr3:uid="{12CF6A16-CD02-4DAF-9CAF-8961CB8BFF41}" name="svm4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,152 +625,301 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
-  <dimension ref="G5:J26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="7:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="2" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="7:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="H7" t="s">
+      <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="I7" t="s">
+      <c r="C17" t="s">
         <v>2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="D17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="7:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="7:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G19" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G20" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H26" s="1"/>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G6:J6"/>
+  <mergeCells count="6">
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A15:G15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalização da geração de resultados para o espectro visível.
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6F24AE-AA4B-4046-B44A-E19D8C0AAEF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFDAB63-E589-45EF-8D63-FE0B52DE482E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>imagem</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>0.9813</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>roi + bag</t>
   </si>
 </sst>
 </file>
@@ -373,6 +379,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,12 +400,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
@@ -884,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,35 +908,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="17" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="17" t="s">
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1170,43 +1176,43 @@
       <c r="D14" s="12"/>
       <c r="E14" s="6"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="22"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="17" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="17" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1238,115 +1244,203 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20">
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="J18">
+        <v>0.97519999999999996</v>
+      </c>
+      <c r="L18" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18">
+        <v>0.70809999999999995</v>
+      </c>
+      <c r="N18" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18">
+        <v>0.99380000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10">
+        <v>1.2500000000000001E-2</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G19" s="10">
+        <v>0.98760000000000003</v>
+      </c>
+      <c r="J19">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="L19">
+        <v>0.98140000000000005</v>
+      </c>
+      <c r="M19">
+        <v>0.97519999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10">
+        <v>3.73E-2</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G20" s="10">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10">
+        <v>3.7699999999999997E-2</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G21" s="10">
+        <v>0.99370000000000003</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="10"/>
+      <c r="D22" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10">
+        <v>2.5000000000000001E-2</v>
+      </c>
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G23" s="10">
+        <v>0.97519999999999996</v>
+      </c>
+      <c r="J23">
+        <v>0.96889999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10">
+        <v>2.53E-2</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="10">
+        <v>0.98729999999999996</v>
+      </c>
+      <c r="J24">
+        <v>0.99370000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="10"/>
+      <c r="D25" s="10">
+        <v>3.7499999999999999E-2</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G25" s="10">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="10"/>
+      <c r="D26" s="10">
+        <v>2.47E-2</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="10">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="21"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="26"/>
+      <c r="D27" s="22">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E27" s="21"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="27"/>
+      <c r="G27" s="22">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
- Adição KNN para imagens originais - Geraçao de Resultados KNN para imagens originais - Versionamento de PS1 para gerenciamento de imagens
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFDAB63-E589-45EF-8D63-FE0B52DE482E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39FAE12-6E65-485B-A957-589CF4019EE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
+    <workbookView xWindow="-28920" yWindow="7065" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>imagem</t>
   </si>
@@ -181,12 +181,6 @@
   </si>
   <si>
     <t>0.9813</t>
-  </si>
-  <si>
-    <t>ROI</t>
-  </si>
-  <si>
-    <t>roi + bag</t>
   </si>
 </sst>
 </file>
@@ -890,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,7 +968,9 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>0.93130000000000002</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4" t="s">
         <v>33</v>
@@ -994,7 +990,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>0.94379999999999997</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4" t="s">
         <v>34</v>
@@ -1014,7 +1012,9 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B6" s="5">
+        <v>0.96879999999999999</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4" t="s">
         <v>35</v>
@@ -1034,7 +1034,9 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
+      <c r="B7" s="5">
+        <v>0.95650000000000002</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4" t="s">
         <v>36</v>
@@ -1054,7 +1056,9 @@
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>0.95630000000000004</v>
+      </c>
       <c r="C8" s="6"/>
       <c r="D8" s="4" t="s">
         <v>37</v>
@@ -1074,7 +1078,9 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5">
+        <v>0.96250000000000002</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4" t="s">
         <v>38</v>
@@ -1094,7 +1100,9 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5">
+        <v>0.9375</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4" t="s">
         <v>32</v>
@@ -1114,7 +1122,9 @@
       <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>0.96250000000000002</v>
+      </c>
       <c r="C11" s="6"/>
       <c r="D11" s="4" t="s">
         <v>32</v>
@@ -1134,7 +1144,9 @@
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5">
+        <v>0.98129999999999995</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4" t="s">
         <v>39</v>
@@ -1154,7 +1166,9 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="7">
+        <v>0.95030000000000003</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9" t="s">
         <v>40</v>
@@ -1212,7 +1226,7 @@
       <c r="I16" s="24"/>
       <c r="J16" s="25"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1244,11 +1258,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="18"/>
+      <c r="B18" s="18">
+        <v>0.92549999999999999</v>
+      </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20">
         <v>1.2500000000000001E-2</v>
@@ -1261,24 +1277,14 @@
       <c r="J18">
         <v>0.97519999999999996</v>
       </c>
-      <c r="L18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M18">
-        <v>0.70809999999999995</v>
-      </c>
-      <c r="N18" t="s">
-        <v>51</v>
-      </c>
-      <c r="O18">
-        <v>0.99380000000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1">
+        <v>0.88819999999999999</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="10">
         <v>1.2500000000000001E-2</v>
@@ -1291,18 +1297,14 @@
       <c r="J19">
         <v>0.98140000000000005</v>
       </c>
-      <c r="L19">
-        <v>0.98140000000000005</v>
-      </c>
-      <c r="M19">
-        <v>0.97519999999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="1"/>
+      <c r="B20" s="1">
+        <v>0.98140000000000005</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="10">
         <v>3.73E-2</v>
@@ -1316,11 +1318,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1">
+        <v>0.9748</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="10">
         <v>3.7699999999999997E-2</v>
@@ -1334,11 +1338,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>0.96250000000000002</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="10">
         <v>2.5000000000000001E-2</v>
@@ -1352,11 +1358,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="1"/>
+      <c r="B23" s="1">
+        <v>0.95030000000000003</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="10">
         <v>2.5000000000000001E-2</v>
@@ -1370,11 +1378,13 @@
         <v>0.96889999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>0.92410000000000003</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="10">
         <v>2.53E-2</v>
@@ -1388,11 +1398,13 @@
         <v>0.99370000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>0.96879999999999999</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="10">
         <v>3.7499999999999999E-2</v>
@@ -1406,11 +1418,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>0.98770000000000002</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="10">
         <v>2.47E-2</v>
@@ -1424,11 +1438,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="21"/>
+      <c r="B27" s="21">
+        <v>0.95630000000000004</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="22">
         <v>1.2500000000000001E-2</v>

</xml_diff>

<commit_message>
Conclusão geração resultados KNN
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39FAE12-6E65-485B-A957-589CF4019EE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CF3372-F4AD-416F-A86A-CF1781BF65F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7065" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>imagem</t>
   </si>
@@ -123,39 +123,6 @@
     <t>20_L_V_L_W</t>
   </si>
   <si>
-    <t>0.9938</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>0.0750</t>
-  </si>
-  <si>
-    <t>0.2250</t>
-  </si>
-  <si>
-    <t>0.1000</t>
-  </si>
-  <si>
-    <t>0.1750</t>
-  </si>
-  <si>
-    <t>0.0683</t>
-  </si>
-  <si>
-    <t>0.1250</t>
-  </si>
-  <si>
-    <t>0.1125</t>
-  </si>
-  <si>
-    <t>0.0125</t>
-  </si>
-  <si>
-    <t>0.1242</t>
-  </si>
-  <si>
     <t>knn3</t>
   </si>
   <si>
@@ -169,18 +136,6 @@
   </si>
   <si>
     <t>Pré-processamento + Otimização</t>
-  </si>
-  <si>
-    <t>0.9875</t>
-  </si>
-  <si>
-    <t>0.9688</t>
-  </si>
-  <si>
-    <t>0.9750</t>
-  </si>
-  <si>
-    <t>0.9813</t>
   </si>
 </sst>
 </file>
@@ -343,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -354,7 +309,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -371,14 +325,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -399,53 +352,56 @@
     <cellStyle name="Célula de Verificação" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -482,55 +438,53 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
-      <border diagonalUp="0" diagonalDown="0">
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
-      <border diagonalUp="0" diagonalDown="0">
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right/>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
   </dxfs>
@@ -554,15 +508,15 @@
   </sortState>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9CD6EEAF-D605-4188-A062-2821793F7914}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{2134A55D-67F8-4BDE-B2FF-785EF61F65A6}" name="knn" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{3887058B-F545-4BEC-89FF-1A68324FCC0A}" name="tree"/>
-    <tableColumn id="4" xr3:uid="{3CE57E63-AE1A-4E11-9613-94E7EEAAA591}" name="svm" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{EE35EF4B-7DC7-4E69-86C3-451405342ABC}" name="knn2" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{7433D010-4521-40A5-BA92-1C0C0211473F}" name="tree2"/>
-    <tableColumn id="7" xr3:uid="{6B5FDDCA-D14F-4A1D-B8C4-0EED1F96B1C6}" name="svm2" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{A581D9AB-270D-4B29-9E91-44E6EF2423A4}" name="knn3" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{C2008561-0E06-46B8-A9E8-4367826B9B57}" name="tree3" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{2AA5EB45-A8E5-4D1F-B1B3-78B36ED46C37}" name="svm3" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2134A55D-67F8-4BDE-B2FF-785EF61F65A6}" name="knn" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{3887058B-F545-4BEC-89FF-1A68324FCC0A}" name="tree" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{3CE57E63-AE1A-4E11-9613-94E7EEAAA591}" name="svm" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{EE35EF4B-7DC7-4E69-86C3-451405342ABC}" name="knn2" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{7433D010-4521-40A5-BA92-1C0C0211473F}" name="tree2" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{6B5FDDCA-D14F-4A1D-B8C4-0EED1F96B1C6}" name="svm2" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{A581D9AB-270D-4B29-9E91-44E6EF2423A4}" name="knn3" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{C2008561-0E06-46B8-A9E8-4367826B9B57}" name="tree3" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{2AA5EB45-A8E5-4D1F-B1B3-78B36ED46C37}" name="svm3" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -573,15 +527,15 @@
   <autoFilter ref="A17:J27" xr:uid="{A4D6B217-4FA4-492C-B809-283D4AF18196}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{3F452B61-5A75-45E9-9A13-8B91CFACB1DC}" name="imagem"/>
-    <tableColumn id="2" xr3:uid="{976E893C-B9F7-4EEC-A16F-C2E9FFF30F2F}" name="knn" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D14D8346-425C-40B6-B42B-FF1859D4CE3D}" name="tree"/>
-    <tableColumn id="4" xr3:uid="{8274C832-A46C-4DE3-9834-744DEE26EE73}" name="svm" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{FC6B0AC5-A94A-4C18-B07C-D85146BDD985}" name="knn2" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{4A16D61D-48DA-477C-A3AA-B1EC58872B63}" name="tree2"/>
-    <tableColumn id="7" xr3:uid="{EC6E9147-7E78-46A9-B7A0-0AEDF0754605}" name="svm2" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{D0C5FBE1-7644-45FC-9C15-3C0B42C36E5C}" name="knn3"/>
-    <tableColumn id="9" xr3:uid="{E0803764-7F93-4571-AB22-E1250CB86649}" name="tree3"/>
-    <tableColumn id="10" xr3:uid="{4774BB1A-C90A-433D-BDDC-79A1CE804D3D}" name="svm3"/>
+    <tableColumn id="2" xr3:uid="{976E893C-B9F7-4EEC-A16F-C2E9FFF30F2F}" name="knn" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{D14D8346-425C-40B6-B42B-FF1859D4CE3D}" name="tree" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{8274C832-A46C-4DE3-9834-744DEE26EE73}" name="svm" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{FC6B0AC5-A94A-4C18-B07C-D85146BDD985}" name="knn2" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{4A16D61D-48DA-477C-A3AA-B1EC58872B63}" name="tree2" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{EC6E9147-7E78-46A9-B7A0-0AEDF0754605}" name="svm2" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{D0C5FBE1-7644-45FC-9C15-3C0B42C36E5C}" name="knn3" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{E0803764-7F93-4571-AB22-E1250CB86649}" name="tree3" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{4774BB1A-C90A-433D-BDDC-79A1CE804D3D}" name="svm3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -886,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC40A39D-D364-4758-95CE-901EFF32DB05}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,35 +856,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -949,63 +903,71 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="10" t="s">
-        <v>44</v>
+      <c r="J3" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>0.93130000000000002</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="4" t="s">
-        <v>31</v>
+      <c r="C4" s="6"/>
+      <c r="D4" s="4">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="3">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>0.94379999999999997</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="4" t="s">
-        <v>46</v>
+      <c r="C5" s="6"/>
+      <c r="D5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.98129999999999995</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="3">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="4">
+        <v>0.98750000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1015,19 +977,23 @@
       <c r="B6" s="5">
         <v>0.96879999999999999</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="4" t="s">
-        <v>49</v>
+      <c r="C6" s="6"/>
+      <c r="D6" s="4">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E6" s="5">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="3">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="4">
+        <v>0.98129999999999995</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1038,18 +1004,22 @@
         <v>0.95650000000000002</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="5"/>
+      <c r="D7" s="4">
+        <v>6.83E-2</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="4" t="s">
-        <v>31</v>
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,18 +1030,22 @@
         <v>0.95630000000000004</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="5"/>
+      <c r="D8" s="4">
+        <v>0.125</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.99380000000000002</v>
+      </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="4" t="s">
-        <v>46</v>
+      <c r="G8" s="3">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="4">
+        <v>0.98750000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1081,19 +1055,23 @@
       <c r="B9" s="5">
         <v>0.96250000000000002</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="4" t="s">
-        <v>31</v>
+      <c r="C9" s="6"/>
+      <c r="D9" s="4">
+        <v>0.1125</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="3">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1103,19 +1081,23 @@
       <c r="B10" s="5">
         <v>0.9375</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="4" t="s">
-        <v>30</v>
+      <c r="C10" s="6"/>
+      <c r="D10" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="3">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="4">
+        <v>0.99380000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1126,18 +1108,22 @@
         <v>0.96250000000000002</v>
       </c>
       <c r="C11" s="6"/>
-      <c r="D11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="5"/>
+      <c r="D11" s="4">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="4" t="s">
-        <v>31</v>
+      <c r="G11" s="3">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1147,19 +1133,23 @@
       <c r="B12" s="5">
         <v>0.98129999999999995</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="4" t="s">
-        <v>31</v>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="3">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1169,62 +1159,66 @@
       <c r="B13" s="7">
         <v>0.95030000000000003</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="9" t="s">
-        <v>31</v>
+      <c r="C13" s="18"/>
+      <c r="D13" s="8">
+        <v>0.1242</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <v>1</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="12"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="6"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="23" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1243,38 +1237,44 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G17" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="I17" t="s">
         <v>10</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="15">
         <v>0.92549999999999999</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20">
+      <c r="C18" s="16"/>
+      <c r="D18" s="17">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20">
+      <c r="E18" s="15">
+        <v>0.97519999999999996</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17">
         <v>0.96889999999999998</v>
       </c>
-      <c r="J18">
+      <c r="H18" s="20">
+        <v>0.96889999999999998</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20">
         <v>0.97519999999999996</v>
       </c>
     </row>
@@ -1282,19 +1282,25 @@
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="5">
         <v>0.88819999999999999</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="10">
+      <c r="C19" s="6"/>
+      <c r="D19" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="10">
+      <c r="E19" s="5">
         <v>0.98760000000000003</v>
       </c>
-      <c r="J19">
+      <c r="F19" s="6"/>
+      <c r="G19" s="3">
+        <v>0.98760000000000003</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0.97519999999999996</v>
+      </c>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20">
         <v>0.98140000000000005</v>
       </c>
     </row>
@@ -1302,19 +1308,25 @@
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="5">
         <v>0.98140000000000005</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="10">
+      <c r="C20" s="6"/>
+      <c r="D20" s="3">
         <v>3.73E-2</v>
       </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="10">
-        <v>1</v>
-      </c>
-      <c r="J20">
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1322,19 +1334,25 @@
       <c r="A21" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="5">
         <v>0.9748</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="10">
+      <c r="C21" s="6"/>
+      <c r="D21" s="3">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="10">
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="3">
         <v>0.99370000000000003</v>
       </c>
-      <c r="J21" s="10">
+      <c r="H21" s="20">
+        <v>1</v>
+      </c>
+      <c r="I21" s="20"/>
+      <c r="J21" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1342,19 +1360,25 @@
       <c r="A22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="5">
         <v>0.96250000000000002</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="10">
+      <c r="C22" s="6"/>
+      <c r="D22" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="10">
-        <v>1</v>
-      </c>
-      <c r="J22">
+      <c r="E22" s="5">
+        <v>1</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="3">
+        <v>1</v>
+      </c>
+      <c r="H22" s="20">
+        <v>1</v>
+      </c>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1362,19 +1386,25 @@
       <c r="A23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="5">
         <v>0.95030000000000003</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="10">
+      <c r="C23" s="6"/>
+      <c r="D23" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="10">
+      <c r="E23" s="5">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="3">
         <v>0.97519999999999996</v>
       </c>
-      <c r="J23">
+      <c r="H23" s="20">
+        <v>0.95030000000000003</v>
+      </c>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20">
         <v>0.96889999999999998</v>
       </c>
     </row>
@@ -1382,19 +1412,25 @@
       <c r="A24" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="5">
         <v>0.92410000000000003</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="10">
+      <c r="C24" s="6"/>
+      <c r="D24" s="3">
         <v>2.53E-2</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="10">
+      <c r="E24" s="5">
+        <v>0.97470000000000001</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="3">
         <v>0.98729999999999996</v>
       </c>
-      <c r="J24">
+      <c r="H24" s="20">
+        <v>0.97470000000000001</v>
+      </c>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20">
         <v>0.99370000000000003</v>
       </c>
     </row>
@@ -1402,19 +1438,25 @@
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="5">
         <v>0.96879999999999999</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="10">
+      <c r="C25" s="6"/>
+      <c r="D25" s="3">
         <v>3.7499999999999999E-2</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="10">
-        <v>0.99380000000000002</v>
-      </c>
-      <c r="J25">
+      <c r="E25" s="5">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="3">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1422,19 +1464,25 @@
       <c r="A26" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="5">
         <v>0.98770000000000002</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="10">
+      <c r="C26" s="6"/>
+      <c r="D26" s="3">
         <v>2.47E-2</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="10">
-        <v>1</v>
-      </c>
-      <c r="J26">
+      <c r="E26" s="5">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+      <c r="H26" s="20">
+        <v>1</v>
+      </c>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1442,19 +1490,25 @@
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="21">
+      <c r="B27" s="7">
         <v>0.95630000000000004</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="22">
+      <c r="C27" s="18"/>
+      <c r="D27" s="19">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="22">
-        <v>0.99380000000000002</v>
-      </c>
-      <c r="J27">
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="H27" s="20">
+        <v>1</v>
+      </c>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checkpoint antes de iniciar crossval
</commit_message>
<xml_diff>
--- a/Estatisticas.xlsx
+++ b/Estatisticas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pontificia Universidade Catolica de Goias\TCC\Projeto\saim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CF3372-F4AD-416F-A86A-CF1781BF65F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC96D7F2-1213-4F5C-AC34-37991EFC23D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7065" windowWidth="29040" windowHeight="15840" xr2:uid="{1A60F312-342B-41F9-A9B7-569E4D5C368D}"/>
   </bookViews>
@@ -841,7 +841,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,14 +925,18 @@
       <c r="B4" s="5">
         <v>0.93130000000000002</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="6">
+        <v>0.375</v>
+      </c>
       <c r="D4" s="4">
         <v>0.22500000000000001</v>
       </c>
       <c r="E4" s="5">
         <v>0.98750000000000004</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6">
+        <v>0.33129999999999998</v>
+      </c>
       <c r="G4" s="3">
         <v>0.99380000000000002</v>
       </c>
@@ -951,14 +955,18 @@
       <c r="B5" s="5">
         <v>0.94379999999999997</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="6">
+        <v>0.41249999999999998</v>
+      </c>
       <c r="D5" s="4">
         <v>0.1</v>
       </c>
       <c r="E5" s="5">
         <v>0.98129999999999995</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6">
+        <v>0.28129999999999999</v>
+      </c>
       <c r="G5" s="3">
         <v>0.96879999999999999</v>
       </c>
@@ -977,14 +985,18 @@
       <c r="B6" s="5">
         <v>0.96879999999999999</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="6">
+        <v>0.41880000000000001</v>
+      </c>
       <c r="D6" s="4">
         <v>0.17499999999999999</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6">
+        <v>0.28129999999999999</v>
+      </c>
       <c r="G6" s="3">
         <v>0.97499999999999998</v>
       </c>
@@ -1003,7 +1015,9 @@
       <c r="B7" s="5">
         <v>0.95650000000000002</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6">
+        <v>0.31059999999999999</v>
+      </c>
       <c r="D7" s="4">
         <v>6.83E-2</v>
       </c>
@@ -1029,7 +1043,9 @@
       <c r="B8" s="5">
         <v>0.95630000000000004</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>0.25</v>
+      </c>
       <c r="D8" s="4">
         <v>0.125</v>
       </c>
@@ -1055,7 +1071,9 @@
       <c r="B9" s="5">
         <v>0.96250000000000002</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>0.43130000000000002</v>
+      </c>
       <c r="D9" s="4">
         <v>0.1125</v>
       </c>
@@ -1081,7 +1099,9 @@
       <c r="B10" s="5">
         <v>0.9375</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6">
+        <v>0.41880000000000001</v>
+      </c>
       <c r="D10" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -1107,7 +1127,9 @@
       <c r="B11" s="5">
         <v>0.96250000000000002</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <v>0.39379999999999998</v>
+      </c>
       <c r="D11" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -1133,7 +1155,9 @@
       <c r="B12" s="5">
         <v>0.98129999999999995</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="6">
+        <v>0.38129999999999997</v>
+      </c>
       <c r="D12" s="4">
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1159,7 +1183,9 @@
       <c r="B13" s="7">
         <v>0.95030000000000003</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="18">
+        <v>0.32950000000000002</v>
+      </c>
       <c r="D13" s="8">
         <v>0.1242</v>
       </c>
@@ -1259,7 +1285,9 @@
       <c r="B18" s="15">
         <v>0.92549999999999999</v>
       </c>
-      <c r="C18" s="16"/>
+      <c r="C18" s="16">
+        <v>0.39129999999999998</v>
+      </c>
       <c r="D18" s="17">
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1285,7 +1313,9 @@
       <c r="B19" s="5">
         <v>0.88819999999999999</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="6">
+        <v>0.4224</v>
+      </c>
       <c r="D19" s="3">
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1311,7 +1341,9 @@
       <c r="B20" s="5">
         <v>0.98140000000000005</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="6">
+        <v>0.4037</v>
+      </c>
       <c r="D20" s="3">
         <v>3.73E-2</v>
       </c>
@@ -1337,7 +1369,9 @@
       <c r="B21" s="5">
         <v>0.9748</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6">
+        <v>0.32079999999999997</v>
+      </c>
       <c r="D21" s="3">
         <v>3.7699999999999997E-2</v>
       </c>
@@ -1363,7 +1397,9 @@
       <c r="B22" s="5">
         <v>0.96250000000000002</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="6">
+        <v>0.28129999999999999</v>
+      </c>
       <c r="D22" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1389,7 +1425,9 @@
       <c r="B23" s="5">
         <v>0.95030000000000003</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="6">
+        <v>0.3851</v>
+      </c>
       <c r="D23" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1415,7 +1453,9 @@
       <c r="B24" s="5">
         <v>0.92410000000000003</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="6">
+        <v>0.43669999999999998</v>
+      </c>
       <c r="D24" s="3">
         <v>2.53E-2</v>
       </c>
@@ -1441,7 +1481,9 @@
       <c r="B25" s="5">
         <v>0.96879999999999999</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="6">
+        <v>0.45629999999999998</v>
+      </c>
       <c r="D25" s="3">
         <v>3.7499999999999999E-2</v>
       </c>
@@ -1467,7 +1509,9 @@
       <c r="B26" s="5">
         <v>0.98770000000000002</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="6">
+        <v>0.30249999999999999</v>
+      </c>
       <c r="D26" s="3">
         <v>2.47E-2</v>
       </c>
@@ -1493,7 +1537,9 @@
       <c r="B27" s="7">
         <v>0.95630000000000004</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="18">
+        <v>0.38129999999999997</v>
+      </c>
       <c r="D27" s="19">
         <v>1.2500000000000001E-2</v>
       </c>

</xml_diff>